<commit_message>
Changed to cucumber Reports
</commit_message>
<xml_diff>
--- a/docs/Testing Charters.xlsx
+++ b/docs/Testing Charters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://testingcircle-my.sharepoint.com/personal/tsturgeon_spartaglobal_com/Documents/Academy/PostGraduation/Project2WebTestFrameWork/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="161" documentId="8_{61BE0308-B044-4E99-9C76-A82CA21F8FB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E0E64495-09B5-4F1B-97EB-6C9FFAC218F1}"/>
+  <xr:revisionPtr revIDLastSave="175" documentId="8_{61BE0308-B044-4E99-9C76-A82CA21F8FB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{43FE8C2E-9FB9-4EA2-80B1-689D6002BA04}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="31650" yWindow="2850" windowWidth="14400" windowHeight="7275" activeTab="2" xr2:uid="{4F92F025-D336-4F87-AB79-14548B9E0CC1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{4F92F025-D336-4F87-AB79-14548B9E0CC1}"/>
   </bookViews>
   <sheets>
     <sheet name="Templates" sheetId="3" r:id="rId1"/>
@@ -579,7 +579,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -597,19 +597,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -618,17 +630,23 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -975,13 +993,13 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.81640625" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -997,7 +1015,7 @@
       <c r="I2" s="14"/>
       <c r="J2" s="14"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1009,7 +1027,7 @@
       <c r="I3" s="14"/>
       <c r="J3" s="14"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1027,7 +1045,7 @@
       </c>
       <c r="J4" s="14"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1039,7 +1057,7 @@
       <c r="I5" s="14"/>
       <c r="J5" s="14"/>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1054,7 +1072,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1069,7 +1087,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="10" t="s">
         <v>6</v>
       </c>
@@ -1081,7 +1099,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="11"/>
       <c r="C9" s="6"/>
       <c r="E9" t="s">
@@ -1091,7 +1109,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="11"/>
       <c r="C10" s="7"/>
       <c r="E10" t="s">
@@ -1101,127 +1119,127 @@
         <v>101</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="11"/>
       <c r="C11" s="6"/>
       <c r="E11" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="11"/>
       <c r="C12" s="6"/>
       <c r="E12" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="11"/>
       <c r="C13" s="6"/>
       <c r="E13" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="11"/>
       <c r="C14" s="6"/>
       <c r="E14" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="11"/>
       <c r="C15" s="6"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="11"/>
       <c r="C16" s="6"/>
       <c r="E16" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="11"/>
       <c r="C17" s="6"/>
       <c r="E17" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="11"/>
       <c r="C18" s="7"/>
       <c r="E18" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="11"/>
       <c r="C19" s="6"/>
       <c r="E19" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="11"/>
       <c r="C20" s="6"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="11"/>
       <c r="C21" s="6"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="11"/>
       <c r="C22" s="6"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="11"/>
       <c r="C23" s="6"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="11"/>
       <c r="C24" s="6"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="11"/>
       <c r="C25" s="7"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="11"/>
       <c r="C26" s="6"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="11"/>
       <c r="C27" s="6"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="11"/>
       <c r="C28" s="6"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="11"/>
       <c r="C29" s="6"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="11"/>
       <c r="C30" s="6"/>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" s="12"/>
       <c r="C31" s="9"/>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C32" s="1"/>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C33" s="3"/>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
         <v>31</v>
       </c>
@@ -1241,21 +1259,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{771601C8-48C6-4AF6-B8A1-1FABAC1EA7EA}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="B2:F72"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C34"/>
+    <sheetView topLeftCell="B33" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37:G73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="101.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="101.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="106" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="101.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1269,7 +1290,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1283,7 +1304,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1297,7 +1318,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1311,7 +1332,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1325,7 +1346,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1339,7 +1360,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="10" t="s">
         <v>6</v>
       </c>
@@ -1353,7 +1374,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="11"/>
       <c r="C9" s="6" t="s">
         <v>12</v>
@@ -1363,7 +1384,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="11"/>
       <c r="C10" s="7" t="s">
         <v>20</v>
@@ -1373,7 +1394,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="11"/>
       <c r="C11" s="6" t="s">
         <v>14</v>
@@ -1383,7 +1404,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="11"/>
       <c r="C12" s="6" t="s">
         <v>15</v>
@@ -1393,7 +1414,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="11"/>
       <c r="C13" s="6" t="s">
         <v>16</v>
@@ -1403,7 +1424,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="11"/>
       <c r="C14" s="6" t="s">
         <v>17</v>
@@ -1413,7 +1434,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="11"/>
       <c r="C15" s="6" t="s">
         <v>18</v>
@@ -1423,7 +1444,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="11"/>
       <c r="C16" s="6" t="s">
         <v>13</v>
@@ -1433,7 +1454,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="11"/>
       <c r="C17" s="6" t="s">
         <v>19</v>
@@ -1443,7 +1464,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="11"/>
       <c r="C18" s="7" t="s">
         <v>24</v>
@@ -1453,7 +1474,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="11"/>
       <c r="C19" s="6" t="s">
         <v>14</v>
@@ -1463,7 +1484,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="11"/>
       <c r="C20" s="6" t="s">
         <v>15</v>
@@ -1473,7 +1494,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="11"/>
       <c r="C21" s="6" t="s">
         <v>16</v>
@@ -1483,21 +1504,23 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="11"/>
       <c r="C22" s="6" t="s">
         <v>21</v>
       </c>
       <c r="E22" s="11"/>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="F22" s="11"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="11"/>
       <c r="C23" s="6" t="s">
         <v>22</v>
       </c>
       <c r="E23" s="11"/>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="F23" s="11"/>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="11"/>
       <c r="C24" s="6" t="s">
         <v>23</v>
@@ -1505,7 +1528,7 @@
       <c r="E24" s="11"/>
       <c r="F24" s="6"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="11"/>
       <c r="C25" s="7" t="s">
         <v>25</v>
@@ -1513,7 +1536,7 @@
       <c r="E25" s="11"/>
       <c r="F25" s="7"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="11"/>
       <c r="C26" s="6" t="s">
         <v>14</v>
@@ -1521,7 +1544,7 @@
       <c r="E26" s="11"/>
       <c r="F26" s="6"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="11"/>
       <c r="C27" s="6" t="s">
         <v>15</v>
@@ -1529,7 +1552,7 @@
       <c r="E27" s="11"/>
       <c r="F27" s="6"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="11"/>
       <c r="C28" s="6" t="s">
         <v>16</v>
@@ -1537,7 +1560,7 @@
       <c r="E28" s="11"/>
       <c r="F28" s="6"/>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="11"/>
       <c r="C29" s="6" t="s">
         <v>17</v>
@@ -1545,7 +1568,7 @@
       <c r="E29" s="11"/>
       <c r="F29" s="6"/>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="11"/>
       <c r="C30" s="6" t="s">
         <v>18</v>
@@ -1553,7 +1576,7 @@
       <c r="E30" s="11"/>
       <c r="F30" s="6"/>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" s="12"/>
       <c r="C31" s="9" t="s">
         <v>26</v>
@@ -1561,7 +1584,7 @@
       <c r="E31" s="12"/>
       <c r="F31" s="9"/>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
         <v>27</v>
       </c>
@@ -1575,7 +1598,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
         <v>28</v>
       </c>
@@ -1589,7 +1612,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
         <v>31</v>
       </c>
@@ -1601,7 +1624,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38" s="10" t="s">
         <v>0</v>
       </c>
@@ -1615,7 +1638,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39" s="10" t="s">
         <v>1</v>
       </c>
@@ -1629,7 +1652,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B40" s="12"/>
       <c r="C40" s="9" t="s">
         <v>46</v>
@@ -1637,7 +1660,7 @@
       <c r="E40" s="12"/>
       <c r="F40" s="9"/>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B41" s="12" t="s">
         <v>2</v>
       </c>
@@ -1651,7 +1674,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
         <v>3</v>
       </c>
@@ -1665,7 +1688,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
         <v>4</v>
       </c>
@@ -1679,7 +1702,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B44" s="1" t="s">
         <v>5</v>
       </c>
@@ -1693,7 +1716,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B45" s="10" t="s">
         <v>6</v>
       </c>
@@ -1707,7 +1730,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B46" s="11"/>
       <c r="C46" s="6" t="s">
         <v>48</v>
@@ -1717,7 +1740,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B47" s="11"/>
       <c r="C47" s="6" t="s">
         <v>17</v>
@@ -1727,7 +1750,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B48" s="11"/>
       <c r="C48" s="6" t="s">
         <v>18</v>
@@ -1737,7 +1760,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B49" s="11"/>
       <c r="C49" s="7" t="s">
         <v>45</v>
@@ -1747,7 +1770,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B50" s="11"/>
       <c r="C50" s="6" t="s">
         <v>49</v>
@@ -1757,7 +1780,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B51" s="11"/>
       <c r="C51" s="6" t="s">
         <v>50</v>
@@ -1767,7 +1790,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B52" s="11"/>
       <c r="C52" s="6" t="s">
         <v>51</v>
@@ -1777,7 +1800,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B53" s="11"/>
       <c r="C53" s="6" t="s">
         <v>52</v>
@@ -1787,7 +1810,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B54" s="11"/>
       <c r="C54" s="6" t="s">
         <v>53</v>
@@ -1797,7 +1820,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B55" s="11"/>
       <c r="C55" s="6" t="s">
         <v>54</v>
@@ -1807,7 +1830,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B56" s="11"/>
       <c r="C56" s="6" t="s">
         <v>55</v>
@@ -1817,7 +1840,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B57" s="11"/>
       <c r="C57" s="7" t="s">
         <v>46</v>
@@ -1827,7 +1850,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B58" s="11"/>
       <c r="C58" s="6" t="s">
         <v>50</v>
@@ -1837,7 +1860,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B59" s="11"/>
       <c r="C59" s="6" t="s">
         <v>56</v>
@@ -1847,7 +1870,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B60" s="11"/>
       <c r="C60" s="6" t="s">
         <v>57</v>
@@ -1857,7 +1880,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B61" s="11"/>
       <c r="C61" s="6" t="s">
         <v>58</v>
@@ -1867,7 +1890,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B62" s="11"/>
       <c r="C62" s="7"/>
       <c r="E62" s="11"/>
@@ -1875,7 +1898,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B63" s="11"/>
       <c r="C63" s="6"/>
       <c r="E63" s="11"/>
@@ -1883,7 +1906,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B64" s="11"/>
       <c r="C64" s="6"/>
       <c r="E64" s="11"/>
@@ -1891,7 +1914,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B65" s="11"/>
       <c r="C65" s="6"/>
       <c r="E65" s="11"/>
@@ -1899,7 +1922,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B66" s="11"/>
       <c r="C66" s="6"/>
       <c r="E66" s="11"/>
@@ -1907,7 +1930,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B67" s="11"/>
       <c r="C67" s="6"/>
       <c r="E67" s="11"/>
@@ -1915,7 +1938,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B68" s="11"/>
       <c r="C68" s="6"/>
       <c r="E68" s="5"/>
@@ -1923,7 +1946,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B69" s="8"/>
       <c r="C69" s="12"/>
       <c r="E69" s="8"/>
@@ -1931,7 +1954,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B70" s="12" t="s">
         <v>27</v>
       </c>
@@ -1945,7 +1968,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B71" s="1" t="s">
         <v>28</v>
       </c>
@@ -1959,7 +1982,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B72" s="1" t="s">
         <v>31</v>
       </c>
@@ -1979,237 +2002,251 @@
     <hyperlink ref="F71" r:id="rId4" display="https://bookcart.azurewebsites.net/register page" xr:uid="{C4D08523-9FDF-43DA-854A-20342E3F4E27}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <pageSetup paperSize="9" scale="44" orientation="landscape" r:id="rId5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{501F9F55-939A-4143-9710-CA573CF79EA6}">
-  <dimension ref="B2:G19"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B2:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="184" zoomScaleNormal="184" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="H21" sqref="A1:H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="7" width="10.6328125" customWidth="1"/>
+    <col min="2" max="7" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B2" s="15" t="s">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="15" t="s">
+      <c r="C2" s="23"/>
+      <c r="D2" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="16"/>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B3" s="17">
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="23"/>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="18">
         <v>1</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="17" t="s">
+      <c r="C3" s="20"/>
+      <c r="D3" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="18"/>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B4" s="15" t="s">
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="20"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="15" t="s">
+      <c r="C4" s="23"/>
+      <c r="D4" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="E4" s="16"/>
-      <c r="F4" s="15" t="s">
+      <c r="E4" s="23"/>
+      <c r="F4" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="G4" s="16"/>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B5" s="20">
+      <c r="G4" s="23"/>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="24">
         <v>45799</v>
       </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="17" t="s">
+      <c r="C5" s="25"/>
+      <c r="D5" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="18"/>
-      <c r="F5" s="17" t="s">
+      <c r="E5" s="20"/>
+      <c r="F5" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="G5" s="18"/>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B6" s="15" t="s">
+      <c r="G5" s="20"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="15" t="s">
+      <c r="C6" s="23"/>
+      <c r="D6" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="E6" s="16"/>
-      <c r="F6" s="15" t="s">
+      <c r="E6" s="23"/>
+      <c r="F6" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="G6" s="16"/>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B7" s="17" t="s">
+      <c r="G6" s="23"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="17" t="s">
+      <c r="C7" s="20"/>
+      <c r="D7" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="E7" s="18"/>
-      <c r="F7" s="17" t="s">
+      <c r="E7" s="20"/>
+      <c r="F7" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="G7" s="18"/>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B8" s="15" t="s">
+      <c r="G7" s="20"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="15" t="s">
+      <c r="C8" s="22"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="F8" s="19"/>
-      <c r="G8" s="16"/>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B9" s="22" t="s">
+      <c r="F8" s="22"/>
+      <c r="G8" s="23"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="C9" s="23"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="22" t="s">
+      <c r="C9" s="16"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="F9" s="23"/>
-      <c r="G9" s="24"/>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B10" s="22"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="24"/>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B11" s="15" t="s">
+      <c r="F9" s="16"/>
+      <c r="G9" s="17"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="15"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="17"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="16"/>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B12" s="22" t="s">
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="23"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="24"/>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B13" s="22" t="s">
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="17"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="24"/>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B14" s="22" t="s">
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="17"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="24"/>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B15" s="22" t="s">
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="17"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="24"/>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B16" s="22" t="s">
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="17"/>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="24"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B17" s="17" t="s">
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="17"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="18"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B18" s="15" t="s">
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="20"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="16"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B19" s="17" t="s">
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="23"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="18"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="28"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="29"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
     <mergeCell ref="B14:G14"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="D7:E7"/>
@@ -2218,20 +2255,18 @@
     <mergeCell ref="E8:G8"/>
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="E9:G9"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="B19:G20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>